<commit_message>
found little mistake in smiles codes which inducded wrong data in descriptors and hca
</commit_message>
<xml_diff>
--- a/Descriptors.xlsx
+++ b/Descriptors.xlsx
@@ -2125,148 +2125,148 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>9.471188586545729</v>
+        <v>5.507494567271353</v>
       </c>
       <c r="C3" t="n">
-        <v>9.471188586545729</v>
+        <v>5.507494567271353</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5016849332325523</v>
+        <v>0.6440460443436633</v>
       </c>
       <c r="E3" t="n">
-        <v>-2.496043083900227</v>
+        <v>-2.022856355505165</v>
       </c>
       <c r="F3" t="n">
-        <v>0.5509088909723503</v>
+        <v>0.4690255384985064</v>
       </c>
       <c r="G3" t="n">
-        <v>11.91666666666667</v>
+        <v>11.92857142857143</v>
       </c>
       <c r="H3" t="n">
-        <v>246.359</v>
+        <v>274.413</v>
       </c>
       <c r="I3" t="n">
-        <v>231.239</v>
+        <v>255.261</v>
       </c>
       <c r="J3" t="n">
-        <v>245.99717935</v>
+        <v>274.028479478</v>
       </c>
       <c r="K3" t="n">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2442462620874037</v>
+        <v>0.2468426025619926</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.3374534836869922</v>
+        <v>-0.3219679757054398</v>
       </c>
       <c r="O3" t="n">
-        <v>0.3374534836869922</v>
+        <v>0.3219679757054398</v>
       </c>
       <c r="P3" t="n">
-        <v>0.2442462620874037</v>
+        <v>0.2468426025619926</v>
       </c>
       <c r="Q3" t="n">
-        <v>1.416666666666667</v>
+        <v>1.071428571428571</v>
       </c>
       <c r="R3" t="n">
-        <v>2.083333333333333</v>
+        <v>1.642857142857143</v>
       </c>
       <c r="S3" t="n">
-        <v>2.583333333333333</v>
+        <v>2.071428571428572</v>
       </c>
       <c r="T3" t="n">
-        <v>32.9210960156317</v>
+        <v>32.92115427442042</v>
       </c>
       <c r="U3" t="n">
-        <v>10.90711199770047</v>
+        <v>10.90606161098254</v>
       </c>
       <c r="V3" t="n">
-        <v>2.117319939358755</v>
+        <v>2.1729804028189</v>
       </c>
       <c r="W3" t="n">
-        <v>-2.121805222714882</v>
+        <v>-2.190680104542174</v>
       </c>
       <c r="X3" t="n">
-        <v>2.553439283776612</v>
+        <v>2.603105594315437</v>
       </c>
       <c r="Y3" t="n">
-        <v>-1.882068243096738</v>
+        <v>-1.938755943544446</v>
       </c>
       <c r="Z3" t="n">
-        <v>8.672111510461773</v>
+        <v>8.675076046216581</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.3405407303004827</v>
+        <v>0.2804267459244999</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.98113945423353</v>
+        <v>2.134451442561562</v>
       </c>
       <c r="AC3" t="n">
-        <v>3.406167136851513</v>
+        <v>3.776797252983614</v>
       </c>
       <c r="AD3" t="n">
-        <v>153.728624104675</v>
+        <v>167.9693269174992</v>
       </c>
       <c r="AE3" t="n">
-        <v>9.449747468305834</v>
+        <v>10.86396103067893</v>
       </c>
       <c r="AF3" t="n">
-        <v>7.355847477601559</v>
+        <v>9.023988953752012</v>
       </c>
       <c r="AG3" t="n">
-        <v>10.69976441138465</v>
+        <v>12.36790588753511</v>
       </c>
       <c r="AH3" t="n">
-        <v>5.621320343559644</v>
+        <v>6.681980515339465</v>
       </c>
       <c r="AI3" t="n">
-        <v>3.816636658257514</v>
+        <v>4.79499275987393</v>
       </c>
       <c r="AJ3" t="n">
-        <v>9.235022810857384</v>
+        <v>10.17852728414391</v>
       </c>
       <c r="AK3" t="n">
-        <v>1.916477366660878</v>
+        <v>2.312909769600933</v>
       </c>
       <c r="AL3" t="n">
-        <v>9.609755970147507</v>
+        <v>10.13633420366469</v>
       </c>
       <c r="AM3" t="n">
-        <v>0.9784701481695968</v>
+        <v>1.255622677552617</v>
       </c>
       <c r="AN3" t="n">
-        <v>6.543137525645594</v>
+        <v>7.976868250331396</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.5563034422005663</v>
+        <v>0.7803654957880988</v>
       </c>
       <c r="AP3" t="n">
-        <v>5.135936201006754</v>
+        <v>6.642842515024668</v>
       </c>
       <c r="AQ3" t="n">
         <v>1.27</v>
       </c>
       <c r="AR3" t="n">
-        <v>330.8502888569996</v>
+        <v>986.1165664634418</v>
       </c>
       <c r="AS3" t="n">
-        <v>13.27</v>
+        <v>15.27</v>
       </c>
       <c r="AT3" t="n">
-        <v>7.653224420022501</v>
+        <v>9.492720917643227</v>
       </c>
       <c r="AU3" t="n">
-        <v>7.895428005704306</v>
+        <v>7.547184073764443</v>
       </c>
       <c r="AV3" t="n">
-        <v>87.75980310045021</v>
+        <v>100.8089988065543</v>
       </c>
       <c r="AW3" t="n">
-        <v>9.417158764464293</v>
+        <v>9.047494323423635</v>
       </c>
       <c r="AX3" t="n">
         <v>0</v>
@@ -2299,16 +2299,16 @@
         <v>18.30546199580378</v>
       </c>
       <c r="BH3" t="n">
-        <v>24.48344689507606</v>
+        <v>31.40718409476669</v>
       </c>
       <c r="BI3" t="n">
         <v>11.50570721349358</v>
       </c>
       <c r="BJ3" t="n">
-        <v>6.606881964512918</v>
+        <v>13.21376392902584</v>
       </c>
       <c r="BK3" t="n">
-        <v>9.417158764464293</v>
+        <v>9.047494323423635</v>
       </c>
       <c r="BL3" t="n">
         <v>40.64400343492098</v>
@@ -2323,10 +2323,10 @@
         <v>0</v>
       </c>
       <c r="BP3" t="n">
-        <v>13.84747439938125</v>
+        <v>20.77121159907187</v>
       </c>
       <c r="BQ3" t="n">
-        <v>23.86544278475328</v>
+        <v>30.4723247492662</v>
       </c>
       <c r="BR3" t="n">
         <v>0</v>
@@ -2350,16 +2350,16 @@
         <v>28.83714734628233</v>
       </c>
       <c r="BY3" t="n">
-        <v>28.75885438750576</v>
+        <v>30.4723247492662</v>
       </c>
       <c r="BZ3" t="n">
-        <v>16.33060325035046</v>
+        <v>20.85435041206228</v>
       </c>
       <c r="CA3" t="n">
         <v>0</v>
       </c>
       <c r="CB3" t="n">
-        <v>13.84747439938125</v>
+        <v>20.77121159907187</v>
       </c>
       <c r="CC3" t="n">
         <v>0</v>
@@ -2374,13 +2374,13 @@
         <v>0</v>
       </c>
       <c r="CG3" t="n">
-        <v>29.46</v>
+        <v>18.46</v>
       </c>
       <c r="CH3" t="n">
         <v>5.693537600778055</v>
       </c>
       <c r="CI3" t="n">
-        <v>4.893411602752475</v>
+        <v>0</v>
       </c>
       <c r="CJ3" t="n">
         <v>0</v>
@@ -2389,43 +2389,43 @@
         <v>0</v>
       </c>
       <c r="CL3" t="n">
-        <v>6.606881964512918</v>
+        <v>13.21376392902584</v>
       </c>
       <c r="CM3" t="n">
         <v>17.25856082024037</v>
       </c>
       <c r="CN3" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO3" t="n">
         <v>11.38172479611316</v>
       </c>
-      <c r="CO3" t="n">
-        <v>0</v>
-      </c>
       <c r="CP3" t="n">
-        <v>18.68562214908174</v>
+        <v>25.60935934877237</v>
       </c>
       <c r="CQ3" t="n">
         <v>6.923737199690624</v>
       </c>
       <c r="CR3" t="n">
-        <v>16.33060325035046</v>
+        <v>20.85435041206228</v>
       </c>
       <c r="CS3" t="n">
-        <v>5.044716789493576</v>
+        <v>11.01498913454271</v>
       </c>
       <c r="CT3" t="n">
-        <v>8.122791241496598</v>
+        <v>8.968239795918366</v>
       </c>
       <c r="CU3" t="n">
-        <v>9.471188586545729</v>
+        <v>0</v>
       </c>
       <c r="CV3" t="n">
         <v>0</v>
       </c>
       <c r="CW3" t="n">
-        <v>-2.496043083900227</v>
+        <v>-2.022856355505165</v>
       </c>
       <c r="CX3" t="n">
-        <v>3.030726095993953</v>
+        <v>3.307730694129504</v>
       </c>
       <c r="CY3" t="n">
         <v>0</v>
@@ -2434,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="DA3" t="n">
-        <v>4.465509259259259</v>
+        <v>7.370785619803477</v>
       </c>
       <c r="DB3" t="n">
         <v>0</v>
@@ -2443,10 +2443,10 @@
         <v>1</v>
       </c>
       <c r="DD3" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="DE3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DF3" t="n">
         <v>2</v>
@@ -2470,16 +2470,16 @@
         <v>0</v>
       </c>
       <c r="DM3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="DN3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DO3" t="n">
         <v>6</v>
       </c>
       <c r="DP3" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="DQ3" t="n">
         <v>0</v>
@@ -2494,10 +2494,10 @@
         <v>0</v>
       </c>
       <c r="DU3" t="n">
-        <v>2.726000000000001</v>
+        <v>3.770200000000003</v>
       </c>
       <c r="DV3" t="n">
-        <v>63.58680000000004</v>
+        <v>72.99400000000004</v>
       </c>
       <c r="DW3" t="n">
         <v>0</v>

</xml_diff>